<commit_message>
added Graphs + conclusion
</commit_message>
<xml_diff>
--- a/query6.xlsx
+++ b/query6.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frede\Documents\GitHub\Casus-DBMS-performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F527C4-42DC-47F2-BD96-DA2525FDFE26}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6841C8-4870-4949-86F5-3CC5A94FAD9A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -101,6 +102,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-BE"/>
+              <a:t>Uitvoertijd</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="nl-BE" baseline="0"/>
+              <a:t> query 6</a:t>
+            </a:r>
+            <a:endParaRPr lang="nl-BE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1035,6 +1066,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>385969</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>27671</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A94E92AC-0B93-4D79-8296-92DB5A1BD72C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1287780" y="381000"/>
+          <a:ext cx="4584589" cy="2755631"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1334,8 +1414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1374,4 +1454,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C4A6FEB-A8F5-4D1F-B959-6073A099CA52}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>